<commit_message>
change to 31 nucleotide difference
</commit_message>
<xml_diff>
--- a/app/home/drscan.xlsx
+++ b/app/home/drscan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="464">
   <si>
     <t>rs356168</t>
   </si>
@@ -1413,13 +1413,16 @@
   </si>
   <si>
     <t>SNPS</t>
+  </si>
+  <si>
+    <t>INDEL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1434,6 +1437,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1468,10 +1477,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1749,88 +1759,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A463"/>
+  <dimension ref="A1:C462"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A428" workbookViewId="0">
+      <selection activeCell="A448" sqref="A448:XFD448"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="36.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="C2">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3992,81 +4016,76 @@
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A460" t="s">
-        <v>458</v>
+      <c r="A460" s="2" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A461" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A462" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="463" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A463" s="2" t="s">
         <v>461</v>
       </c>
     </row>

</xml_diff>